<commit_message>
country groups continuation; quadratic regression cont.
</commit_message>
<xml_diff>
--- a/output/results_2023-08-08/preprocessed/ind_coef_product_amount_per_capita_vs_time.xlsx
+++ b/output/results_2023-08-08/preprocessed/ind_coef_product_amount_per_capita_vs_time.xlsx
@@ -675,7 +675,7 @@
         <v>-1.2367438e-05</v>
       </c>
       <c r="G2" t="n">
-        <v>-0.882372404551</v>
+        <v>-0.882372404556</v>
       </c>
       <c r="H2" t="n">
         <v>0.000899202868</v>
@@ -855,7 +855,7 @@
         <v>-2.709755e-06</v>
       </c>
       <c r="G3" t="n">
-        <v>-1.111575521965</v>
+        <v>-1.111575521963</v>
       </c>
       <c r="H3" t="n">
         <v>0.001118784552</v>
@@ -1215,7 +1215,7 @@
         <v>-2.600455e-06</v>
       </c>
       <c r="G5" t="n">
-        <v>-0.568459036747</v>
+        <v>-0.568459036746</v>
       </c>
       <c r="H5" t="n">
         <v>0.000573326051</v>
@@ -1395,7 +1395,7 @@
         <v>-1.41355e-07</v>
       </c>
       <c r="G6" t="n">
-        <v>0.137448058498</v>
+        <v>0.137448058496</v>
       </c>
       <c r="H6" t="n">
         <v>-0.000137298251</v>
@@ -1575,7 +1575,7 @@
         <v>-5.07622e-07</v>
       </c>
       <c r="G7" t="n">
-        <v>-0.438403870702</v>
+        <v>-0.438403870701</v>
       </c>
       <c r="H7" t="n">
         <v>0.000440629397</v>
@@ -1755,7 +1755,7 @@
         <v>1.856142e-06</v>
       </c>
       <c r="G8" t="n">
-        <v>-0.144138363249</v>
+        <v>-0.14413836325</v>
       </c>
       <c r="H8" t="n">
         <v>0.000142944057</v>
@@ -2115,7 +2115,7 @@
         <v>-4.197183e-06</v>
       </c>
       <c r="G10" t="n">
-        <v>0.069039142177</v>
+        <v>0.069039142175</v>
       </c>
       <c r="H10" t="n">
         <v>-6.4770126e-05</v>
@@ -2461,7 +2461,7 @@
         <v>1.843171e-06</v>
       </c>
       <c r="G12" t="n">
-        <v>-0.641453063629</v>
+        <v>-0.641453063628</v>
       </c>
       <c r="H12" t="n">
         <v>0.00064250122</v>
@@ -2641,7 +2641,7 @@
         <v>-2.697595e-06</v>
       </c>
       <c r="G13" t="n">
-        <v>-6.799141809469</v>
+        <v>-6.79914180946</v>
       </c>
       <c r="H13" t="n">
         <v>0.006784972266</v>
@@ -2771,7 +2771,7 @@
         <v>-0.000258504092</v>
       </c>
       <c r="G14" t="n">
-        <v>13.22726952796</v>
+        <v>13.227269527858</v>
       </c>
       <c r="H14" t="n">
         <v>-0.01301061635</v>
@@ -2951,7 +2951,7 @@
         <v>-4.302435e-06</v>
       </c>
       <c r="G15" t="n">
-        <v>-0.087769419519</v>
+        <v>-0.08776941952</v>
       </c>
       <c r="H15" t="n">
         <v>9.2656852e-05</v>
@@ -3131,7 +3131,7 @@
         <v>1.113447e-06</v>
       </c>
       <c r="G16" t="n">
-        <v>-0.024303171018</v>
+        <v>-0.02430317102</v>
       </c>
       <c r="H16" t="n">
         <v>2.3670857e-05</v>
@@ -3311,7 +3311,7 @@
         <v>8.460405e-06</v>
       </c>
       <c r="G17" t="n">
-        <v>0.590217585141</v>
+        <v>0.590217585137</v>
       </c>
       <c r="H17" t="n">
         <v>-0.000600268157</v>
@@ -3491,7 +3491,7 @@
         <v>-5.123782e-06</v>
       </c>
       <c r="G18" t="n">
-        <v>-0.212635282037</v>
+        <v>-0.212635282039</v>
       </c>
       <c r="H18" t="n">
         <v>0.000218912965</v>
@@ -3671,7 +3671,7 @@
         <v>3.099354e-06</v>
       </c>
       <c r="G19" t="n">
-        <v>0.325024274446</v>
+        <v>0.325024274445</v>
       </c>
       <c r="H19" t="n">
         <v>-0.000329274383</v>
@@ -4031,7 +4031,7 @@
         <v>1.092648e-06</v>
       </c>
       <c r="G21" t="n">
-        <v>0.290859026264</v>
+        <v>0.290859026262</v>
       </c>
       <c r="H21" t="n">
         <v>-0.000292277598</v>
@@ -4197,7 +4197,7 @@
         <v>-3.127824e-06</v>
       </c>
       <c r="G22" t="n">
-        <v>0.27882208554</v>
+        <v>0.278822085536</v>
       </c>
       <c r="H22" t="n">
         <v>-0.000275876851</v>
@@ -4377,7 +4377,7 @@
         <v>1.2028466e-05</v>
       </c>
       <c r="G23" t="n">
-        <v>-1.488389069988</v>
+        <v>-1.488389069987</v>
       </c>
       <c r="H23" t="n">
         <v>0.001482670771</v>
@@ -4557,7 +4557,7 @@
         <v>-2.250337e-06</v>
       </c>
       <c r="G24" t="n">
-        <v>0.080063136435</v>
+        <v>0.080063136434</v>
       </c>
       <c r="H24" t="n">
         <v>-7.755095499999999e-05</v>
@@ -4737,7 +4737,7 @@
         <v>-5.955648e-06</v>
       </c>
       <c r="G25" t="n">
-        <v>0.15152267708</v>
+        <v>0.151522677079</v>
       </c>
       <c r="H25" t="n">
         <v>-0.000145861779</v>
@@ -4917,7 +4917,7 @@
         <v>-2.515612e-06</v>
       </c>
       <c r="G26" t="n">
-        <v>0.144314531733</v>
+        <v>0.144314531732</v>
       </c>
       <c r="H26" t="n">
         <v>-0.000142186654</v>
@@ -5277,7 +5277,7 @@
         <v>-4.248628e-06</v>
       </c>
       <c r="G28" t="n">
-        <v>0.115457617897</v>
+        <v>0.115457617895</v>
       </c>
       <c r="H28" t="n">
         <v>-0.00011118622</v>
@@ -5443,7 +5443,7 @@
         <v>-3.77739e-07</v>
       </c>
       <c r="G29" t="n">
-        <v>0.211774659514</v>
+        <v>0.211774659513</v>
       </c>
       <c r="H29" t="n">
         <v>-0.00021171838</v>
@@ -5609,7 +5609,7 @@
         <v>3.198476e-06</v>
       </c>
       <c r="G30" t="n">
-        <v>-0.207068121543</v>
+        <v>-0.207068121544</v>
       </c>
       <c r="H30" t="n">
         <v>0.000203712458</v>
@@ -5751,7 +5751,7 @@
         <v>-2.249986e-06</v>
       </c>
       <c r="G31" t="n">
-        <v>0.83672918045</v>
+        <v>0.836729180448</v>
       </c>
       <c r="H31" t="n">
         <v>-0.000836029584</v>
@@ -5917,7 +5917,7 @@
         <v>-8.69123e-07</v>
       </c>
       <c r="G32" t="n">
-        <v>1.494031340137</v>
+        <v>1.494031340135</v>
       </c>
       <c r="H32" t="n">
         <v>-0.001496077764</v>
@@ -20480,7 +20480,7 @@
         <v>1.266106e-06</v>
       </c>
       <c r="G11" t="n">
-        <v>-0.115778176602</v>
+        <v>-0.115778176603</v>
       </c>
       <c r="H11" t="n">
         <v>0.000115235574</v>
@@ -21083,7 +21083,7 @@
         <v>-1.728766e-06</v>
       </c>
       <c r="G14" t="n">
-        <v>-1.449687842817</v>
+        <v>-1.449687842811</v>
       </c>
       <c r="H14" t="n">
         <v>0.001446021408</v>
@@ -21411,7 +21411,7 @@
         <v>1.781239e-06</v>
       </c>
       <c r="G16" t="n">
-        <v>-0.198843060554</v>
+        <v>-0.198843060555</v>
       </c>
       <c r="H16" t="n">
         <v>0.000198335523</v>
@@ -21612,7 +21612,7 @@
         <v>1.0980154e-05</v>
       </c>
       <c r="G17" t="n">
-        <v>-0.170952503767</v>
+        <v>-0.170952503768</v>
       </c>
       <c r="H17" t="n">
         <v>0.000161291833</v>
@@ -22416,7 +22416,7 @@
         <v>3.507668e-06</v>
       </c>
       <c r="G21" t="n">
-        <v>-0.481882740066</v>
+        <v>-0.481882740067</v>
       </c>
       <c r="H21" t="n">
         <v>0.00048137845</v>
@@ -22816,7 +22816,7 @@
         <v>3.2854909e-05</v>
       </c>
       <c r="G23" t="n">
-        <v>-2.782825841667</v>
+        <v>-2.782825841674</v>
       </c>
       <c r="H23" t="n">
         <v>0.002767251983</v>
@@ -23017,7 +23017,7 @@
         <v>1.6339673e-05</v>
       </c>
       <c r="G24" t="n">
-        <v>-1.319545285497</v>
+        <v>-1.3195452855</v>
       </c>
       <c r="H24" t="n">
         <v>0.001311510037</v>
@@ -23419,7 +23419,7 @@
         <v>1.030741e-06</v>
       </c>
       <c r="G26" t="n">
-        <v>-1.083791563686</v>
+        <v>-1.083791563688</v>
       </c>
       <c r="H26" t="n">
         <v>0.001089228535</v>
@@ -23620,7 +23620,7 @@
         <v>1.926126e-06</v>
       </c>
       <c r="G27" t="n">
-        <v>-0.334399494871</v>
+        <v>-0.334399494872</v>
       </c>
       <c r="H27" t="n">
         <v>0.00033452091</v>
@@ -24480,7 +24480,7 @@
         <v>8.7381e-07</v>
       </c>
       <c r="G33" t="n">
-        <v>-0.054422837303</v>
+        <v>-0.054422837298</v>
       </c>
       <c r="H33" t="n">
         <v>5.321599e-05</v>
@@ -25237,7 +25237,7 @@
         <v>5.89232e-07</v>
       </c>
       <c r="G2" t="n">
-        <v>-0.981309416847</v>
+        <v>-0.981309416849</v>
       </c>
       <c r="H2" t="n">
         <v>0.000986932433</v>
@@ -25438,7 +25438,7 @@
         <v>-2.053407e-06</v>
       </c>
       <c r="G3" t="n">
-        <v>-1.157484016574</v>
+        <v>-1.157484016575</v>
       </c>
       <c r="H3" t="n">
         <v>0.001166471999</v>
@@ -25639,7 +25639,7 @@
         <v>-1.721923e-06</v>
       </c>
       <c r="G4" t="n">
-        <v>-1.263996758658</v>
+        <v>-1.263996758661</v>
       </c>
       <c r="H4" t="n">
         <v>0.001273319975</v>
@@ -25840,7 +25840,7 @@
         <v>-2.44994e-06</v>
       </c>
       <c r="G5" t="n">
-        <v>-0.118959756585</v>
+        <v>-0.118959756584</v>
       </c>
       <c r="H5" t="n">
         <v>0.000122495974</v>
@@ -26242,7 +26242,7 @@
         <v>5.276339e-06</v>
       </c>
       <c r="G7" t="n">
-        <v>-0.393959360692</v>
+        <v>-0.393959360693</v>
       </c>
       <c r="H7" t="n">
         <v>0.000391426652</v>
@@ -26443,7 +26443,7 @@
         <v>1.0267225e-05</v>
       </c>
       <c r="G8" t="n">
-        <v>-5.080509205102</v>
+        <v>-5.080509205112</v>
       </c>
       <c r="H8" t="n">
         <v>0.005099881242</v>
@@ -26644,7 +26644,7 @@
         <v>4.56193e-06</v>
       </c>
       <c r="G9" t="n">
-        <v>-2.607737433738</v>
+        <v>-2.607737433744</v>
       </c>
       <c r="H9" t="n">
         <v>0.002618511041</v>
@@ -26845,7 +26845,7 @@
         <v>-4.371798e-06</v>
       </c>
       <c r="G10" t="n">
-        <v>-0.580745872305</v>
+        <v>-0.580745872304</v>
       </c>
       <c r="H10" t="n">
         <v>0.000588792234</v>
@@ -27046,7 +27046,7 @@
         <v>6.78984e-06</v>
       </c>
       <c r="G11" t="n">
-        <v>-1.162444973368</v>
+        <v>-1.162444973371</v>
       </c>
       <c r="H11" t="n">
         <v>0.001162742602</v>
@@ -27247,7 +27247,7 @@
         <v>2.55716e-07</v>
       </c>
       <c r="G12" t="n">
-        <v>-1.666295214227</v>
+        <v>-1.66629521423</v>
       </c>
       <c r="H12" t="n">
         <v>0.001676027962</v>
@@ -27448,7 +27448,7 @@
         <v>5.173972e-06</v>
       </c>
       <c r="G13" t="n">
-        <v>1.25303384811</v>
+        <v>1.253033848113</v>
       </c>
       <c r="H13" t="n">
         <v>-0.001265083512</v>
@@ -27649,7 +27649,7 @@
         <v>2.8154524e-05</v>
       </c>
       <c r="G14" t="n">
-        <v>-0.398762884586</v>
+        <v>-0.39876288459</v>
       </c>
       <c r="H14" t="n">
         <v>0.000374188199</v>
@@ -27850,7 +27850,7 @@
         <v>-3.72449e-07</v>
       </c>
       <c r="G15" t="n">
-        <v>-0.893411856459</v>
+        <v>-0.89341185646</v>
       </c>
       <c r="H15" t="n">
         <v>0.000899120964</v>
@@ -28453,7 +28453,7 @@
         <v>5.27238e-07</v>
       </c>
       <c r="G18" t="n">
-        <v>-0.427081053171</v>
+        <v>-0.42708105317</v>
       </c>
       <c r="H18" t="n">
         <v>0.000429360339</v>
@@ -28654,7 +28654,7 @@
         <v>1.0298442e-05</v>
       </c>
       <c r="G19" t="n">
-        <v>-2.319023168477</v>
+        <v>-2.319023168483</v>
       </c>
       <c r="H19" t="n">
         <v>0.00232236662</v>
@@ -28855,7 +28855,7 @@
         <v>-1.480914e-06</v>
       </c>
       <c r="G20" t="n">
-        <v>-0.8784162068269999</v>
+        <v>-0.878416206828</v>
       </c>
       <c r="H20" t="n">
         <v>0.000885266164</v>
@@ -29056,7 +29056,7 @@
         <v>2.921884e-06</v>
       </c>
       <c r="G21" t="n">
-        <v>-1.726922141044</v>
+        <v>-1.726922141047</v>
       </c>
       <c r="H21" t="n">
         <v>0.001734251086</v>
@@ -29257,7 +29257,7 @@
         <v>4.63464e-07</v>
       </c>
       <c r="G22" t="n">
-        <v>-0.620689824712</v>
+        <v>-0.620689824713</v>
       </c>
       <c r="H22" t="n">
         <v>0.000624360847</v>
@@ -29458,7 +29458,7 @@
         <v>-3.00259e-06</v>
       </c>
       <c r="G23" t="n">
-        <v>-0.068307320078</v>
+        <v>-0.06830732007699999</v>
       </c>
       <c r="H23" t="n">
         <v>7.1997795e-05</v>
@@ -29659,7 +29659,7 @@
         <v>-3.576479e-06</v>
       </c>
       <c r="G24" t="n">
-        <v>0.510737098026</v>
+        <v>0.510737098028</v>
       </c>
       <c r="H24" t="n">
         <v>-0.000509712541</v>
@@ -30061,7 +30061,7 @@
         <v>-4.044609e-06</v>
       </c>
       <c r="G26" t="n">
-        <v>-0.098586081917</v>
+        <v>-0.098586081915</v>
       </c>
       <c r="H26" t="n">
         <v>0.000103617927</v>
@@ -30262,7 +30262,7 @@
         <v>-3.131138e-06</v>
       </c>
       <c r="G27" t="n">
-        <v>-0.19041051095</v>
+        <v>-0.190410510949</v>
       </c>
       <c r="H27" t="n">
         <v>0.000195239067</v>
@@ -30865,7 +30865,7 @@
         <v>6.428919e-06</v>
       </c>
       <c r="G30" t="n">
-        <v>1.1500798948</v>
+        <v>1.150079894804</v>
       </c>
       <c r="H30" t="n">
         <v>-0.001162723056</v>
@@ -31066,7 +31066,7 @@
         <v>1.144345e-06</v>
       </c>
       <c r="G31" t="n">
-        <v>-0.9240089254</v>
+        <v>-0.924008925402</v>
       </c>
       <c r="H31" t="n">
         <v>0.000928365142</v>
@@ -31468,7 +31468,7 @@
         <v>-1.680518e-05</v>
       </c>
       <c r="G33" t="n">
-        <v>3.683194728263</v>
+        <v>3.683194728268</v>
       </c>
       <c r="H33" t="n">
         <v>-0.003686486413</v>
@@ -31669,7 +31669,7 @@
         <v>-3.686023e-06</v>
       </c>
       <c r="G34" t="n">
-        <v>-0.014697614342</v>
+        <v>-0.014697614341</v>
       </c>
       <c r="H34" t="n">
         <v>1.8845819e-05</v>
@@ -34872,7 +34872,7 @@
         <v>1.08093e-07</v>
       </c>
       <c r="G9" t="n">
-        <v>-0.030165138444</v>
+        <v>-0.030165138445</v>
       </c>
       <c r="H9" t="n">
         <v>3.0234096e-05</v>
@@ -36852,7 +36852,7 @@
         <v>-3.83204e-07</v>
       </c>
       <c r="G21" t="n">
-        <v>-0.134145530741</v>
+        <v>-0.134145530742</v>
       </c>
       <c r="H21" t="n">
         <v>0.00013426724</v>
@@ -37681,7 +37681,7 @@
         <v>3.721502e-06</v>
       </c>
       <c r="G26" t="n">
-        <v>-0.219335504257</v>
+        <v>-0.219335504258</v>
       </c>
       <c r="H26" t="n">
         <v>0.000217042061</v>
@@ -38083,7 +38083,7 @@
         <v>2.77881e-07</v>
       </c>
       <c r="G28" t="n">
-        <v>-2.428171694138</v>
+        <v>-2.428171694143</v>
       </c>
       <c r="H28" t="n">
         <v>0.00242253316</v>
@@ -38483,7 +38483,7 @@
         <v>1.318859e-06</v>
       </c>
       <c r="G32" t="n">
-        <v>-0.24907533583</v>
+        <v>-0.249075335831</v>
       </c>
       <c r="H32" t="n">
         <v>0.00024721785</v>
@@ -38622,7 +38622,7 @@
         <v>5.0255405e-05</v>
       </c>
       <c r="G33" t="n">
-        <v>7.450472123955</v>
+        <v>7.450472124006</v>
       </c>
       <c r="H33" t="n">
         <v>-0.00752652448</v>
@@ -45635,7 +45635,7 @@
         <v>1.75192e-07</v>
       </c>
       <c r="G2" t="n">
-        <v>-0.046376398017</v>
+        <v>-0.046376398016</v>
       </c>
       <c r="H2" t="n">
         <v>4.6282806e-05</v>
@@ -48631,7 +48631,7 @@
         <v>1.03573e-07</v>
       </c>
       <c r="G24" t="n">
-        <v>0.010145004909</v>
+        <v>0.010145004908</v>
       </c>
       <c r="H24" t="n">
         <v>-1.0260752e-05</v>
@@ -50193,7 +50193,7 @@
         <v>9.68311e-07</v>
       </c>
       <c r="G2" t="n">
-        <v>-0.649690525844</v>
+        <v>-0.649690525842</v>
       </c>
       <c r="H2" t="n">
         <v>0.000645847894</v>
@@ -50323,7 +50323,7 @@
         <v>-3.11142e-07</v>
       </c>
       <c r="G4" t="n">
-        <v>-0.263879362526</v>
+        <v>-0.263879362531</v>
       </c>
       <c r="H4" t="n">
         <v>0.000262961254</v>
@@ -50447,7 +50447,7 @@
         <v>6.64302e-07</v>
       </c>
       <c r="G6" t="n">
-        <v>-0.419756395271</v>
+        <v>-0.419756395248</v>
       </c>
       <c r="H6" t="n">
         <v>0.000417262305</v>
@@ -50605,7 +50605,7 @@
         <v>-9.9553e-08</v>
       </c>
       <c r="G8" t="n">
-        <v>-0.105820531246</v>
+        <v>-0.105820531248</v>
       </c>
       <c r="H8" t="n">
         <v>0.000105424232</v>
@@ -50682,7 +50682,7 @@
         <v>-3.97756e-07</v>
       </c>
       <c r="G9" t="n">
-        <v>-0.212291195814</v>
+        <v>-0.2122911958</v>
       </c>
       <c r="H9" t="n">
         <v>0.000211752318</v>
@@ -50763,7 +50763,7 @@
         <v>-2.88322e-07</v>
       </c>
       <c r="G10" t="n">
-        <v>-0.017371488604</v>
+        <v>-0.0173714886</v>
       </c>
       <c r="H10" t="n">
         <v>1.7601092e-05</v>
@@ -50891,7 +50891,7 @@
         <v>-5.7729e-07</v>
       </c>
       <c r="G12" t="n">
-        <v>0.047709996624</v>
+        <v>0.047709996623</v>
       </c>
       <c r="H12" t="n">
         <v>-4.6911708e-05</v>
@@ -51066,7 +51066,7 @@
         <v>1.378156e-06</v>
       </c>
       <c r="G15" t="n">
-        <v>0.008693918768999999</v>
+        <v>0.008693918768000001</v>
       </c>
       <c r="H15" t="n">
         <v>-1.0009231e-05</v>
@@ -51143,7 +51143,7 @@
         <v>4.2703e-07</v>
       </c>
       <c r="G16" t="n">
-        <v>-0.317766565633</v>
+        <v>-0.317766565634</v>
       </c>
       <c r="H16" t="n">
         <v>0.00031593701</v>
@@ -51299,7 +51299,7 @@
         <v>-8.5074e-08</v>
       </c>
       <c r="G18" t="n">
-        <v>-0.027274382349</v>
+        <v>-0.027274382348</v>
       </c>
       <c r="H18" t="n">
         <v>2.7239279e-05</v>
@@ -51376,7 +51376,7 @@
         <v>2.50906e-07</v>
       </c>
       <c r="G19" t="n">
-        <v>-0.016678694375</v>
+        <v>-0.016678694376</v>
       </c>
       <c r="H19" t="n">
         <v>1.6358087e-05</v>
@@ -51453,7 +51453,7 @@
         <v>-7.82219e-07</v>
       </c>
       <c r="G20" t="n">
-        <v>-0.349535190771</v>
+        <v>-0.349535190765</v>
       </c>
       <c r="H20" t="n">
         <v>0.000348158663</v>
@@ -51670,7 +51670,7 @@
         <v>-2.94339e-07</v>
       </c>
       <c r="G23" t="n">
-        <v>-0.171039078295</v>
+        <v>-0.171039078298</v>
       </c>
       <c r="H23" t="n">
         <v>0.000170544263</v>
@@ -51747,7 +51747,7 @@
         <v>-1.2023e-06</v>
       </c>
       <c r="G24" t="n">
-        <v>0.275255208506</v>
+        <v>0.275255208514</v>
       </c>
       <c r="H24" t="n">
         <v>-0.000272740053</v>
@@ -51824,7 +51824,7 @@
         <v>-3.41673e-07</v>
       </c>
       <c r="G25" t="n">
-        <v>-0.02802134271</v>
+        <v>-0.028021342701</v>
       </c>
       <c r="H25" t="n">
         <v>2.824714e-05</v>
@@ -51905,7 +51905,7 @@
         <v>8.186369999999999e-07</v>
       </c>
       <c r="G26" t="n">
-        <v>-0.628465413612</v>
+        <v>-0.628465413622</v>
       </c>
       <c r="H26" t="n">
         <v>0.000624733467</v>
@@ -51982,7 +51982,7 @@
         <v>-3.30655e-07</v>
       </c>
       <c r="G27" t="n">
-        <v>0.287083327409</v>
+        <v>0.287083327414</v>
       </c>
       <c r="H27" t="n">
         <v>-0.00028539533</v>

</xml_diff>